<commit_message>
latest changes after two merge to master
</commit_message>
<xml_diff>
--- a/src/test/resources/Trackx.truelocate.xlsx
+++ b/src/test/resources/Trackx.truelocate.xlsx
@@ -20,7 +20,7 @@
     <sheet name="Itemclass" sheetId="7" r:id="rId6"/>
     <sheet name="ItemType" sheetId="8" r:id="rId7"/>
     <sheet name="IdentifierType" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
+    <sheet name="LocationList" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>sUsername</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>DOCK</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -968,19 +971,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -988,19 +992,22 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1008,15 +1015,18 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
       </c>
       <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit and Delete flows
</commit_message>
<xml_diff>
--- a/src/test/resources/Trackx.truelocate.xlsx
+++ b/src/test/resources/Trackx.truelocate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="5145" tabRatio="500" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="4695" tabRatio="500" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,27 @@
     <sheet name="ItemType" sheetId="8" r:id="rId7"/>
     <sheet name="IdentifierType" sheetId="9" r:id="rId8"/>
     <sheet name="LocationList" sheetId="11" r:id="rId9"/>
-    <sheet name="Item" sheetId="12" r:id="rId10"/>
-    <sheet name="EditRegion" sheetId="13" r:id="rId11"/>
-    <sheet name="FacilityCreate" sheetId="15" r:id="rId12"/>
-    <sheet name="Provision" sheetId="14" r:id="rId13"/>
+    <sheet name="EditItemclass" sheetId="31" r:id="rId10"/>
+    <sheet name="Item" sheetId="12" r:id="rId11"/>
+    <sheet name="EditRegion" sheetId="13" r:id="rId12"/>
+    <sheet name="EditLocationlist" sheetId="16" r:id="rId13"/>
+    <sheet name="EditIdentifierType" sheetId="17" r:id="rId14"/>
+    <sheet name="EditItemType" sheetId="18" r:id="rId15"/>
+    <sheet name="DeleteRegion" sheetId="32" r:id="rId16"/>
+    <sheet name="FacilityCreate" sheetId="15" r:id="rId17"/>
+    <sheet name="Provision" sheetId="14" r:id="rId18"/>
+    <sheet name="EditItem" sheetId="19" r:id="rId19"/>
+    <sheet name="RegionGlobalfilter" sheetId="20" r:id="rId20"/>
+    <sheet name="DeleteLocationlist" sheetId="21" r:id="rId21"/>
+    <sheet name="DeleteItemclass" sheetId="22" r:id="rId22"/>
+    <sheet name="DeleteIdentifiertype" sheetId="23" r:id="rId23"/>
+    <sheet name="DeleteItemtype" sheetId="24" r:id="rId24"/>
+    <sheet name="FacilityEdit" sheetId="25" r:id="rId25"/>
+    <sheet name="DeleteFacility" sheetId="26" r:id="rId26"/>
+    <sheet name="Sheet12" sheetId="27" r:id="rId27"/>
+    <sheet name="Sheet13" sheetId="28" r:id="rId28"/>
+    <sheet name="Sheet14" sheetId="29" r:id="rId29"/>
+    <sheet name="Sheet15" sheetId="30" r:id="rId30"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="171">
   <si>
     <t>sUsername</t>
   </si>
@@ -125,39 +142,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Jothish@gmail.com</t>
-  </si>
-  <si>
-    <t>Region9894323</t>
-  </si>
-  <si>
-    <t>Name6576724</t>
-  </si>
-  <si>
-    <t>test6733424</t>
-  </si>
-  <si>
-    <t>test661224</t>
-  </si>
-  <si>
-    <t>test6332324</t>
-  </si>
-  <si>
-    <t>test312324</t>
-  </si>
-  <si>
-    <t>test235424</t>
-  </si>
-  <si>
     <t>test431231224</t>
   </si>
   <si>
-    <t>test2316543231</t>
-  </si>
-  <si>
-    <t>test35134324232</t>
-  </si>
-  <si>
     <t xml:space="preserve"> sName</t>
   </si>
   <si>
@@ -173,12 +160,6 @@
     <t>sLocationTypedropdown</t>
   </si>
   <si>
-    <t>Test23123</t>
-  </si>
-  <si>
-    <t>Namer4343</t>
-  </si>
-  <si>
     <t>ACM</t>
   </si>
   <si>
@@ -266,12 +247,6 @@
     <t>sItem</t>
   </si>
   <si>
-    <t>Test3431</t>
-  </si>
-  <si>
-    <t>Nm1431</t>
-  </si>
-  <si>
     <t>sEachweight</t>
   </si>
   <si>
@@ -329,15 +304,9 @@
     <t>BARCODE</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>sValue</t>
   </si>
   <si>
-    <t>Test13432</t>
-  </si>
-  <si>
     <t xml:space="preserve"> sItemdropdown</t>
   </si>
   <si>
@@ -350,119 +319,260 @@
     <t>String sStocknumber</t>
   </si>
   <si>
+    <t>sRegion</t>
+  </si>
+  <si>
+    <t>sFacilityType</t>
+  </si>
+  <si>
+    <t>sApplicationType</t>
+  </si>
+  <si>
+    <t>sAddressLine1</t>
+  </si>
+  <si>
+    <t>sAddressLine2</t>
+  </si>
+  <si>
+    <t>sCity</t>
+  </si>
+  <si>
+    <t>sState</t>
+  </si>
+  <si>
+    <t>sZipCode</t>
+  </si>
+  <si>
+    <t>sCountry</t>
+  </si>
+  <si>
+    <t>sContactName</t>
+  </si>
+  <si>
+    <t>sContact</t>
+  </si>
+  <si>
+    <t>sLatitude</t>
+  </si>
+  <si>
+    <t>sLongitude</t>
+  </si>
+  <si>
+    <t>sGeoFence</t>
+  </si>
+  <si>
+    <t>sVerifiedAddress</t>
+  </si>
+  <si>
+    <t>sInventoryManaged</t>
+  </si>
+  <si>
+    <t>sBillTo</t>
+  </si>
+  <si>
+    <t>sBillToFacility</t>
+  </si>
+  <si>
+    <t>sShipTo</t>
+  </si>
+  <si>
+    <t>sShipFrom</t>
+  </si>
+  <si>
+    <t>sCrossDock</t>
+  </si>
+  <si>
+    <t>sTimeZone</t>
+  </si>
+  <si>
+    <t>sSystemofMeasurement</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>Depot Portal</t>
+  </si>
+  <si>
+    <t>28,30, Kodambakkam High Road, Nungambakkam</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil nadu</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>rb.admin@gmail.com</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>STOCK NUMBER</t>
+  </si>
+  <si>
+    <t>t611076</t>
+  </si>
+  <si>
+    <t>VEHICLE</t>
+  </si>
+  <si>
+    <t>RERE</t>
+  </si>
+  <si>
     <t>ITEM11022017</t>
   </si>
   <si>
-    <t>NAMER4343</t>
-  </si>
-  <si>
-    <t>sRegion</t>
-  </si>
-  <si>
-    <t>sFacilityType</t>
-  </si>
-  <si>
-    <t>sApplicationType</t>
-  </si>
-  <si>
-    <t>sAddressLine1</t>
-  </si>
-  <si>
-    <t>sAddressLine2</t>
-  </si>
-  <si>
-    <t>sCity</t>
-  </si>
-  <si>
-    <t>sState</t>
-  </si>
-  <si>
-    <t>sZipCode</t>
-  </si>
-  <si>
-    <t>sCountry</t>
-  </si>
-  <si>
-    <t>sContactName</t>
-  </si>
-  <si>
-    <t>sContact</t>
-  </si>
-  <si>
-    <t>sLatitude</t>
-  </si>
-  <si>
-    <t>sLongitude</t>
-  </si>
-  <si>
-    <t>sGeoFence</t>
-  </si>
-  <si>
-    <t>sVerifiedAddress</t>
-  </si>
-  <si>
-    <t>sInventoryManaged</t>
-  </si>
-  <si>
-    <t>sBillTo</t>
-  </si>
-  <si>
-    <t>sBillToFacility</t>
-  </si>
-  <si>
-    <t>sShipTo</t>
-  </si>
-  <si>
-    <t>sShipFrom</t>
-  </si>
-  <si>
-    <t>sCrossDock</t>
-  </si>
-  <si>
-    <t>sTimeZone</t>
-  </si>
-  <si>
-    <t>sSystemofMeasurement</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>NAME1416</t>
-  </si>
-  <si>
-    <t>CUSTOMER</t>
-  </si>
-  <si>
-    <t>Depot Portal</t>
-  </si>
-  <si>
-    <t>28,30, Kodambakkam High Road, Nungambakkam</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Tamil nadu</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>ACT</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>TESTREGION7070</t>
+    <t>ASDA</t>
+  </si>
+  <si>
+    <t>T77</t>
+  </si>
+  <si>
+    <t>ADDISON</t>
+  </si>
+  <si>
+    <t>HDFBAD</t>
+  </si>
+  <si>
+    <t>NAMER43435</t>
+  </si>
+  <si>
+    <t>TEST101620171</t>
+  </si>
+  <si>
+    <t>SERIALNO</t>
+  </si>
+  <si>
+    <t>Name60000901</t>
+  </si>
+  <si>
+    <t>FACILITY6000901</t>
+  </si>
+  <si>
+    <t>14ST-02</t>
+  </si>
+  <si>
+    <t>ENTRYCODE11</t>
+  </si>
+  <si>
+    <t>fusion@gmail.com</t>
+  </si>
+  <si>
+    <t>Region20000931656</t>
+  </si>
+  <si>
+    <t>Name200009311398</t>
+  </si>
+  <si>
+    <t>code2000019656412</t>
+  </si>
+  <si>
+    <t>Name20000193124758</t>
+  </si>
+  <si>
+    <t>Test68979535</t>
+  </si>
+  <si>
+    <t>Code3000018566713</t>
+  </si>
+  <si>
+    <t>Name30000182317909</t>
+  </si>
+  <si>
+    <t>Name098074</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Test05454354</t>
+  </si>
+  <si>
+    <t>Test134320</t>
+  </si>
+  <si>
+    <t>14ST-04</t>
+  </si>
+  <si>
+    <t>Test23109808</t>
+  </si>
+  <si>
+    <t>Name353213AB</t>
+  </si>
+  <si>
+    <t>SERIALNO11</t>
+  </si>
+  <si>
+    <t>CLASS3</t>
+  </si>
+  <si>
+    <t>CAR656</t>
+  </si>
+  <si>
+    <t>NAME9890A</t>
+  </si>
+  <si>
+    <t>REGIONDELETE</t>
+  </si>
+  <si>
+    <t>FACILITTYDELETE</t>
+  </si>
+  <si>
+    <t>itemcode90AD</t>
+  </si>
+  <si>
+    <t>Namecode980AD</t>
+  </si>
+  <si>
+    <t>code5425656VB</t>
+  </si>
+  <si>
+    <t>Test535689801CV</t>
+  </si>
+  <si>
+    <t>Name502189NM</t>
+  </si>
+  <si>
+    <t>FACILITY606CMN</t>
+  </si>
+  <si>
+    <t>Name6012AZS</t>
+  </si>
+  <si>
+    <t>Test500ACVB</t>
+  </si>
+  <si>
+    <t>Name50VBN05</t>
+  </si>
+  <si>
+    <t>TEST001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -477,6 +587,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -506,11 +622,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -863,7 +980,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +1000,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -900,10 +1017,57 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +1077,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -922,135 +1086,135 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>65</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>66</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>67</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>78</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AK1" t="s">
         <v>79</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AL1" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AM1" t="s">
         <v>81</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1059,40 +1223,40 @@
         <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="R2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="S2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="U2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="V2">
         <v>2</v>
@@ -1154,12 +1318,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1333,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1180,13 +1344,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1195,15 +1359,203 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1216,111 +1568,114 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="J1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="K1" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="L1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="M1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="N1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="O1" t="s">
         <v>6</v>
       </c>
       <c r="P1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="R1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="S1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="T1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="U1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="V1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="W1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="X1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="Y1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="Z1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="AA1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="J2" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="K2">
         <v>600034</v>
       </c>
       <c r="L2" t="s">
-        <v>136</v>
+        <v>117</v>
+      </c>
+      <c r="O2" t="s">
+        <v>139</v>
       </c>
       <c r="S2" t="s">
         <v>28</v>
@@ -1329,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="W2" t="s">
         <v>28</v>
@@ -1341,10 +1696,10 @@
         <v>28</v>
       </c>
       <c r="Z2" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="AA2" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1352,12 +1707,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,53 +1722,316 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="G2" s="3">
-        <v>4.3241234123412301E+17</v>
+        <v>43241234123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AE2">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>3</v>
+      </c>
+      <c r="AG2">
+        <v>3</v>
+      </c>
+      <c r="AH2">
+        <v>3</v>
+      </c>
+      <c r="AI2">
+        <v>4</v>
+      </c>
+      <c r="AJ2">
+        <v>4</v>
+      </c>
+      <c r="AK2">
+        <v>4</v>
+      </c>
+      <c r="AL2">
+        <v>6</v>
+      </c>
+      <c r="AM2">
+        <v>6</v>
+      </c>
+      <c r="AN2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1506,12 +2124,362 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2">
+        <v>600034</v>
+      </c>
+      <c r="M2" t="s">
+        <v>117</v>
+      </c>
+      <c r="T2" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,13 +2494,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1649,13 +2629,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +2653,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,13 +2674,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +2698,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,10 +2722,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1769,7 +2749,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,45 +2764,45 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ie and firefox browser changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Trackx.truelocate.xlsx
+++ b/src/test/resources/Trackx.truelocate.xlsx
@@ -5,16 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Itemclass" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ItemType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="IdentifierType" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="FacilityCreate" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="FacilityEdit" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="UpdateUser" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="FacilityCreate" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="FacilityEdit" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="UpdateUser" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="IdentifierType" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="FacilityAdvancedFilter" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t xml:space="preserve">sUsername</t>
   </si>
@@ -49,7 +50,133 @@
     <t xml:space="preserve">sDescription</t>
   </si>
   <si>
-    <t xml:space="preserve">test8</t>
+    <t xml:space="preserve">test9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sRegion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sFacilityType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sApplicationType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sZipCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sContactName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sContact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sLatitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sLongitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sGeoFence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sVerifiedAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sInventoryManaged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sBillTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sBillToFacility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sShipTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sShipFrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sCrossDock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sTimeZone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sSystemofMeasurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME1416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUSTOMER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depot Portal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,30, Kodambakkam High Road, Nungambakkam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chennai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil nadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa/Asmara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sFirstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sLastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test11user@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
   </si>
   <si>
     <t xml:space="preserve">sRFID</t>
@@ -58,136 +185,25 @@
     <t xml:space="preserve">sProtocol</t>
   </si>
   <si>
-    <t xml:space="preserve">test12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">test13</t>
   </si>
   <si>
     <t xml:space="preserve">RFCODE</t>
   </si>
   <si>
-    <t xml:space="preserve">sRegion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sFacilityType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sApplicationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sZipCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sContactName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sContact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sEmail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sLatitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sLongitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sGeoFence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sVerifiedAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sInventoryManaged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sBillTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sBillToFacility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sShipTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sShipFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sCrossDock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sTimeZone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sSystemofMeasurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAME1416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUSTOMER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depot Portal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,30, Kodambakkam High Road, Nungambakkam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chennai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamil nadu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Africa/Asmara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sFirstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sLastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test11user@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
+    <t xml:space="preserve">TEST3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil Nadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
 </sst>
 </file>
@@ -198,7 +214,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -301,6 +317,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -450,7 +472,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -460,6 +482,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -709,71 +739,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -812,135 +777,216 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>600034</v>
       </c>
       <c r="L2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -955,87 +1001,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1053,24 +1018,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1085,4 +1050,147 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adv Filter changes for Item, ItemClass, ItemType and Identifier Type screen
</commit_message>
<xml_diff>
--- a/src/test/resources/Trackx.truelocate.xlsx
+++ b/src/test/resources/Trackx.truelocate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,10 @@
     <sheet name="UpdateUser" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="IdentifierType" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="FacilityAdvancedFilter" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ItemclassAdvFilter" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="ItemTypeAdvFilter" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="IdentifierTypeAdvFilter" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="ItemAdvancedFilter" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
   <si>
     <t xml:space="preserve">sUsername</t>
   </si>
@@ -35,7 +39,7 @@
     <t xml:space="preserve">sPassword</t>
   </si>
   <si>
-    <t xml:space="preserve">rb.admin@gmail.com</t>
+    <t xml:space="preserve">balasanthanam92@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Test@123</t>
@@ -204,6 +208,72 @@
   </si>
   <si>
     <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLASS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sIsRFID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sToDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-12-2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-11-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sItemClass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sItemType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sManufacture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sManufactureItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sInventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sInventoryType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSVITEMCODE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSVITEMNAME100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEHICLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toyota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Serialized</t>
   </si>
 </sst>
 </file>
@@ -214,7 +284,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -318,12 +388,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -472,7 +536,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,10 +551,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -588,8 +648,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,6 +689,201 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -637,7 +892,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,11 +1369,14 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1177,11 +1435,60 @@
       <c r="H2" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>